<commit_message>
Program Structure mjor changes
</commit_message>
<xml_diff>
--- a/Model trained results.xlsx
+++ b/Model trained results.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wilson\Data_Analytics\Master in IS Course\Master in IS Course\Internship\git-Grab-MSFT\Grab-MSFT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C5838A-32C1-438C-9400-95655B67894D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1707F933-1043-4448-8397-346E3C707D32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="1164" windowWidth="17736" windowHeight="10908" xr2:uid="{4EFF8A82-8904-4487-97E4-88C9915742B1}"/>
+    <workbookView xWindow="5244" yWindow="0" windowWidth="17736" windowHeight="10908" activeTab="1" xr2:uid="{4EFF8A82-8904-4487-97E4-88C9915742B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Model</t>
   </si>
@@ -106,13 +107,43 @@
   </si>
   <si>
     <t>LSTM1-3in2out_sorted_normalised</t>
+  </si>
+  <si>
+    <t>Val RMSE</t>
+  </si>
+  <si>
+    <t>test RMSE</t>
+  </si>
+  <si>
+    <t>LSTM1-3in2out0</t>
+  </si>
+  <si>
+    <t>LSTM1-3in2out1</t>
+  </si>
+  <si>
+    <t>LSTM1-3in3out0</t>
+  </si>
+  <si>
+    <t>LSTM1-3in3out1</t>
+  </si>
+  <si>
+    <t>Bi-LSTM1-3in2out0</t>
+  </si>
+  <si>
+    <t>Bi-LSTM1-3in2out1</t>
+  </si>
+  <si>
+    <t>Bi-LSTM1-3in3out0</t>
+  </si>
+  <si>
+    <t>Bi-LSTM1-3in3out1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +155,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -477,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB03C19F-158B-4F26-A757-89B624D13BF0}">
   <dimension ref="B2:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:G21"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -955,4 +992,228 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A32C215C-5A50-436A-8BDC-2F31DCDC98A2}">
+  <dimension ref="B2:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="4">
+        <v>771330</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3">
+        <v>2</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="4">
+        <v>771330</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>20</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="4">
+        <v>179202</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3">
+        <v>3</v>
+      </c>
+      <c r="G5" s="3">
+        <v>3</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="4">
+        <v>179202</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="4">
+        <v>3422722</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>20</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3422722</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>20</v>
+      </c>
+      <c r="F8" s="3">
+        <v>3</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="4">
+        <v>859394</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>20</v>
+      </c>
+      <c r="F9" s="3">
+        <v>3</v>
+      </c>
+      <c r="G9" s="3">
+        <v>3</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="4">
+        <v>859394</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>20</v>
+      </c>
+      <c r="F10" s="3">
+        <v>3</v>
+      </c>
+      <c r="G10" s="3">
+        <v>3</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
UPdates in excel file
</commit_message>
<xml_diff>
--- a/Model trained results.xlsx
+++ b/Model trained results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wilson\Data_Analytics\Master in IS Course\Master in IS Course\Internship\git-Grab-MSFT\Grab-MSFT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C66AE5-F049-4256-93DA-5688D601B74D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D79209-1AB3-40A9-8D10-5754F7FB04B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5292" yWindow="72" windowWidth="17736" windowHeight="10908" activeTab="1" xr2:uid="{4EFF8A82-8904-4487-97E4-88C9915742B1}"/>
+    <workbookView xWindow="8520" yWindow="408" windowWidth="13980" windowHeight="10908" activeTab="1" xr2:uid="{4EFF8A82-8904-4487-97E4-88C9915742B1}"/>
   </bookViews>
   <sheets>
     <sheet name="3-2" sheetId="1" r:id="rId1"/>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB03C19F-158B-4F26-A757-89B624D13BF0}">
   <dimension ref="B2:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD16"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -910,7 +910,7 @@
   <dimension ref="B2:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>